<commit_message>
feat: Enhance LPU validation process by adding agency and constructor data loading
- Implemented load_agencies and load_constructors functions to read agency and constructor data from specified file paths.
- Updated validate_lpu function to include loading of agency and constructor data, improving the validation workflow.
- Added error handling for file loading and mandatory column checks in both new functions.
- Refactored existing functions to ensure consistent data transformation and case handling.
- Enhanced logging for better traceability during the validation process.
</commit_message>
<xml_diff>
--- a/data/inputs/agencias/BASE_AGENCIAS.xlsx
+++ b/data/inputs/agencias/BASE_AGENCIAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/agencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C6A8922-D948-4E1B-BC7B-B67061881718}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8036EF31-9BAF-43F8-A7AB-15B8CB23894C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,13 +416,13 @@
     <t>BANCO</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
     <t>ESPAÇO ITAÚ</t>
   </si>
   <si>
     <t>FULL SERVICE</t>
+  </si>
+  <si>
+    <t>TIPO</t>
   </si>
 </sst>
 </file>
@@ -492,6 +492,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,7 +763,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -794,7 +800,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>5</v>
@@ -826,7 +832,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
@@ -858,7 +864,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>18</v>
@@ -890,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
@@ -922,7 +928,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>26</v>
@@ -954,7 +960,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>18</v>
@@ -986,7 +992,7 @@
         <v>33</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>14</v>
@@ -1018,7 +1024,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>18</v>
@@ -1050,7 +1056,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>14</v>
@@ -1082,7 +1088,7 @@
         <v>25</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>26</v>
@@ -1114,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>26</v>
@@ -1146,7 +1152,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>14</v>
@@ -1178,7 +1184,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>18</v>
@@ -1210,7 +1216,7 @@
         <v>33</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>14</v>
@@ -1242,7 +1248,7 @@
         <v>13</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>18</v>
@@ -1274,7 +1280,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>14</v>
@@ -1306,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>26</v>
@@ -1338,7 +1344,7 @@
         <v>13</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>18</v>
@@ -1370,7 +1376,7 @@
         <v>13</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>14</v>
@@ -1402,7 +1408,7 @@
         <v>33</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>14</v>
@@ -1434,7 +1440,7 @@
         <v>25</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>26</v>
@@ -1466,7 +1472,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>14</v>
@@ -1498,7 +1504,7 @@
         <v>13</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>26</v>
@@ -1530,7 +1536,7 @@
         <v>25</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>18</v>
@@ -1562,7 +1568,7 @@
         <v>33</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>18</v>
@@ -1594,7 +1600,7 @@
         <v>13</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>14</v>
@@ -1626,7 +1632,7 @@
         <v>33</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>14</v>
@@ -1658,7 +1664,7 @@
         <v>25</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>18</v>
@@ -1690,7 +1696,7 @@
         <v>13</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>26</v>
@@ -1722,7 +1728,7 @@
         <v>33</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>14</v>
@@ -1754,7 +1760,7 @@
         <v>25</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
feat: Update agency and budget metadata handling with new merge functions and validation
</commit_message>
<xml_diff>
--- a/data/inputs/agencias/BASE_AGENCIAS.xlsx
+++ b/data/inputs/agencias/BASE_AGENCIAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/agencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F715137D-F9E2-4E44-BCA2-97F5B065FF58}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F514FE42-96CF-47AC-9F07-E511B4118D88}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -698,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -712,13 +712,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1007,23 +1001,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="6" customWidth="1"/>
-    <col min="3" max="4" width="11.21875" style="6" customWidth="1"/>
-    <col min="5" max="6" width="11.21875" style="7" customWidth="1"/>
-    <col min="7" max="9" width="11.21875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" style="6" customWidth="1"/>
-    <col min="16" max="17" width="19.21875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="11.21875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="5" customWidth="1"/>
+    <col min="3" max="9" width="11.21875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="5" customWidth="1"/>
+    <col min="16" max="17" width="19.21875" style="5" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1039,10 +1033,10 @@
       <c r="D1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1095,10 +1089,10 @@
       <c r="D2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>-23.543900000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>-46.640999999999998</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1134,7 +1128,7 @@
       <c r="Q2" s="1">
         <v>8119</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="5">
         <v>13</v>
       </c>
     </row>
@@ -1151,10 +1145,10 @@
       <c r="D3" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>-23.561499999999999</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>-46.656300000000002</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1190,13 +1184,13 @@
       <c r="Q3" s="1">
         <v>4126</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1003</v>
+        <v>3149</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -1207,10 +1201,10 @@
       <c r="D4" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>-22.9056</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>-47.0608</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1246,7 +1240,7 @@
       <c r="Q4" s="1">
         <v>2706</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1263,10 +1257,10 @@
       <c r="D5" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>-23.967500000000001</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>-46.334299999999999</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1302,7 +1296,7 @@
       <c r="Q5" s="1">
         <v>6257</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>32</v>
       </c>
     </row>
@@ -1319,10 +1313,10 @@
       <c r="D6" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>-21.177499999999998</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>-47.820799999999998</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1358,13 +1352,13 @@
       <c r="Q6" s="1">
         <v>4251</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1006</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
@@ -1375,10 +1369,10 @@
       <c r="D7" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>-23.691400000000002</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>-46.564599999999999</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1414,7 +1408,7 @@
       <c r="Q7" s="1">
         <v>4520</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="5">
         <v>16</v>
       </c>
     </row>
@@ -1431,10 +1425,10 @@
       <c r="D8" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>-19.938600000000001</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>-43.933399999999999</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1470,7 +1464,7 @@
       <c r="Q8" s="1">
         <v>2244</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1487,10 +1481,10 @@
       <c r="D9" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>-18.9145</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>-48.275399999999998</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1526,7 +1520,7 @@
       <c r="Q9" s="1">
         <v>3384</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1543,10 +1537,10 @@
       <c r="D10" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>-19.938099999999999</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>-44.0366</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1582,7 +1576,7 @@
       <c r="Q10" s="1">
         <v>7564</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="5">
         <v>29</v>
       </c>
     </row>
@@ -1599,10 +1593,10 @@
       <c r="D11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>-9.9747000000000003</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>-67.8249</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1638,7 +1632,7 @@
       <c r="Q11" s="1">
         <v>2589</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11" s="5">
         <v>25</v>
       </c>
     </row>
@@ -1655,10 +1649,10 @@
       <c r="D12" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>-3.0916000000000001</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>-60.0261</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1694,7 +1688,7 @@
       <c r="Q12" s="1">
         <v>8747</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="5">
         <v>33</v>
       </c>
     </row>
@@ -1711,10 +1705,10 @@
       <c r="D13" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>-3.0945</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>-60.024999999999999</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1750,7 +1744,7 @@
       <c r="Q13" s="1">
         <v>6162</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="5">
         <v>21</v>
       </c>
     </row>
@@ -1767,10 +1761,10 @@
       <c r="D14" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>-12.9748</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>-38.5124</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1806,7 +1800,7 @@
       <c r="Q14" s="1">
         <v>8843</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14" s="5">
         <v>22</v>
       </c>
     </row>
@@ -1823,10 +1817,10 @@
       <c r="D15" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>-3.7319</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>-38.499299999999998</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1862,7 +1856,7 @@
       <c r="Q15" s="1">
         <v>5526</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15" s="5">
         <v>32</v>
       </c>
     </row>
@@ -1879,10 +1873,10 @@
       <c r="D16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>-8.1227</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>-34.9026</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1918,7 +1912,7 @@
       <c r="Q16" s="1">
         <v>5949</v>
       </c>
-      <c r="R16" s="6">
+      <c r="R16" s="5">
         <v>18</v>
       </c>
     </row>
@@ -1935,10 +1929,10 @@
       <c r="D17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>-5.8403999999999998</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>-35.206499999999998</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1974,7 +1968,7 @@
       <c r="Q17" s="1">
         <v>2470</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R17" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1991,10 +1985,10 @@
       <c r="D18" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>-25.4405</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>-49.292299999999997</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -2030,7 +2024,7 @@
       <c r="Q18" s="1">
         <v>9146</v>
       </c>
-      <c r="R18" s="6">
+      <c r="R18" s="5">
         <v>29</v>
       </c>
     </row>
@@ -2047,10 +2041,10 @@
       <c r="D19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>-23.304400000000001</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>-51.1691</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -2086,7 +2080,7 @@
       <c r="Q19" s="1">
         <v>8407</v>
       </c>
-      <c r="R19" s="6">
+      <c r="R19" s="5">
         <v>32</v>
       </c>
     </row>
@@ -2103,10 +2097,10 @@
       <c r="D20" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>-27.594899999999999</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>-48.548200000000001</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -2142,7 +2136,7 @@
       <c r="Q20" s="1">
         <v>1675</v>
       </c>
-      <c r="R20" s="6">
+      <c r="R20" s="5">
         <v>18</v>
       </c>
     </row>
@@ -2159,10 +2153,10 @@
       <c r="D21" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>-26.304400000000001</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>-48.8461</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -2198,7 +2192,7 @@
       <c r="Q21" s="1">
         <v>8970</v>
       </c>
-      <c r="R21" s="6">
+      <c r="R21" s="5">
         <v>18</v>
       </c>
     </row>
@@ -2215,10 +2209,10 @@
       <c r="D22" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>-16.6799</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>-49.255000000000003</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -2254,7 +2248,7 @@
       <c r="Q22" s="1">
         <v>6572</v>
       </c>
-      <c r="R22" s="6">
+      <c r="R22" s="5">
         <v>18</v>
       </c>
     </row>
@@ -2271,10 +2265,10 @@
       <c r="D23" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>-20.4697</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>-54.620100000000001</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -2310,7 +2304,7 @@
       <c r="Q23" s="1">
         <v>3514</v>
       </c>
-      <c r="R23" s="6">
+      <c r="R23" s="5">
         <v>4</v>
       </c>
     </row>
@@ -2327,10 +2321,10 @@
       <c r="D24" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>-15.569599999999999</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>-56.073500000000003</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -2366,7 +2360,7 @@
       <c r="Q24" s="1">
         <v>4311</v>
       </c>
-      <c r="R24" s="6">
+      <c r="R24" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2383,10 +2377,10 @@
       <c r="D25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>-15.815</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>-47.897599999999997</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -2422,7 +2416,7 @@
       <c r="Q25" s="1">
         <v>3851</v>
       </c>
-      <c r="R25" s="6">
+      <c r="R25" s="5">
         <v>33</v>
       </c>
     </row>
@@ -2439,10 +2433,10 @@
       <c r="D26" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>-22.8964</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>-43.124600000000001</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -2478,7 +2472,7 @@
       <c r="Q26" s="1">
         <v>526</v>
       </c>
-      <c r="R26" s="6">
+      <c r="R26" s="5">
         <v>9</v>
       </c>
     </row>
@@ -2495,10 +2489,10 @@
       <c r="D27" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>-22.903500000000001</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>-43.1768</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -2534,7 +2528,7 @@
       <c r="Q27" s="1">
         <v>9245</v>
       </c>
-      <c r="R27" s="6">
+      <c r="R27" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2551,10 +2545,10 @@
       <c r="D28" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>-23.001100000000001</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>-43.365400000000001</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -2590,7 +2584,7 @@
       <c r="Q28" s="1">
         <v>8592</v>
       </c>
-      <c r="R28" s="6">
+      <c r="R28" s="5">
         <v>13</v>
       </c>
     </row>
@@ -2607,10 +2601,10 @@
       <c r="D29" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>-22.523399999999999</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>-44.104900000000001</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -2646,7 +2640,7 @@
       <c r="Q29" s="1">
         <v>1146</v>
       </c>
-      <c r="R29" s="6">
+      <c r="R29" s="5">
         <v>11</v>
       </c>
     </row>
@@ -2663,10 +2657,10 @@
       <c r="D30" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>-2.5297000000000001</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>-44.302799999999998</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -2702,7 +2696,7 @@
       <c r="Q30" s="1">
         <v>5761</v>
       </c>
-      <c r="R30" s="6">
+      <c r="R30" s="5">
         <v>29</v>
       </c>
     </row>
@@ -2719,10 +2713,10 @@
       <c r="D31" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>-5.0826000000000002</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <v>-42.802199999999999</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -2758,7 +2752,7 @@
       <c r="Q31" s="1">
         <v>6278</v>
       </c>
-      <c r="R31" s="6">
+      <c r="R31" s="5">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Enhance data processing by adding normalization options and updating settings for agencies and constructors
</commit_message>
<xml_diff>
--- a/data/inputs/agencias/BASE_AGENCIAS.xlsx
+++ b/data/inputs/agencias/BASE_AGENCIAS.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/agencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F514FE42-96CF-47AC-9F07-E511B4118D88}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEE9F5C9-21C7-4DD7-B2C1-00174464546F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$R$31</definedName>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="204">
   <si>
     <t>CD_PONTO</t>
   </si>
@@ -424,9 +423,6 @@
   </si>
   <si>
     <t>QUADRO TOTAL</t>
-  </si>
-  <si>
-    <t>ENDEREÇO</t>
   </si>
   <si>
     <t>CEP</t>
@@ -698,19 +694,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -730,10 +720,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1002,22 +988,22 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="5" customWidth="1"/>
-    <col min="3" max="9" width="11.21875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" style="5" customWidth="1"/>
-    <col min="16" max="17" width="19.21875" style="5" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="11.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="3" customWidth="1"/>
+    <col min="3" max="9" width="11.21875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="3" customWidth="1"/>
+    <col min="16" max="17" width="19.21875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1028,16 +1014,16 @@
         <v>123</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -1061,16 +1047,16 @@
         <v>124</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>127</v>
@@ -1084,15 +1070,15 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>-23.543900000000001</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>-46.640999999999998</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1108,7 +1094,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>126</v>
@@ -1120,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>12</v>
@@ -1128,27 +1114,27 @@
       <c r="Q2" s="1">
         <v>8119</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1002</v>
+        <v>3893</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>-23.561499999999999</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>-46.656300000000002</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1164,7 +1150,7 @@
         <v>21</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>126</v>
@@ -1176,7 +1162,7 @@
         <v>14</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>15</v>
@@ -1184,7 +1170,7 @@
       <c r="Q3" s="1">
         <v>4126</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="3">
         <v>34</v>
       </c>
     </row>
@@ -1196,15 +1182,15 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>-22.9056</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>-47.0608</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1220,7 +1206,7 @@
         <v>21</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>126</v>
@@ -1232,7 +1218,7 @@
         <v>11</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>18</v>
@@ -1240,7 +1226,7 @@
       <c r="Q4" s="1">
         <v>2706</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1252,15 +1238,15 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>-23.967500000000001</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>-46.334299999999999</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1276,7 +1262,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>126</v>
@@ -1288,7 +1274,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>23</v>
@@ -1296,7 +1282,7 @@
       <c r="Q5" s="1">
         <v>6257</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="3">
         <v>32</v>
       </c>
     </row>
@@ -1308,15 +1294,15 @@
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>-21.177499999999998</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>-47.820799999999998</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1332,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>126</v>
@@ -1344,7 +1330,7 @@
         <v>14</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>26</v>
@@ -1352,7 +1338,7 @@
       <c r="Q6" s="1">
         <v>4251</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1364,15 +1350,15 @@
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>-23.691400000000002</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>-46.564599999999999</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1388,7 +1374,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>126</v>
@@ -1400,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>29</v>
@@ -1408,7 +1394,7 @@
       <c r="Q7" s="1">
         <v>4520</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="3">
         <v>16</v>
       </c>
     </row>
@@ -1420,15 +1406,15 @@
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>-19.938600000000001</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>-43.933399999999999</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1444,7 +1430,7 @@
         <v>21</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>126</v>
@@ -1456,7 +1442,7 @@
         <v>14</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>33</v>
@@ -1464,7 +1450,7 @@
       <c r="Q8" s="1">
         <v>2244</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="3">
         <v>40</v>
       </c>
     </row>
@@ -1476,15 +1462,15 @@
         <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>-18.9145</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>-48.275399999999998</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1500,7 +1486,7 @@
         <v>10</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>126</v>
@@ -1512,7 +1498,7 @@
         <v>11</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>36</v>
@@ -1520,7 +1506,7 @@
       <c r="Q9" s="1">
         <v>3384</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="3">
         <v>40</v>
       </c>
     </row>
@@ -1532,15 +1518,15 @@
         <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>-19.938099999999999</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>-44.0366</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1556,7 +1542,7 @@
         <v>10</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>126</v>
@@ -1568,7 +1554,7 @@
         <v>22</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>39</v>
@@ -1576,7 +1562,7 @@
       <c r="Q10" s="1">
         <v>7564</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="3">
         <v>29</v>
       </c>
     </row>
@@ -1588,15 +1574,15 @@
         <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>-9.9747000000000003</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>-67.8249</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1609,10 +1595,10 @@
         <v>43</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>126</v>
@@ -1624,7 +1610,7 @@
         <v>22</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>44</v>
@@ -1632,7 +1618,7 @@
       <c r="Q11" s="1">
         <v>2589</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="3">
         <v>25</v>
       </c>
     </row>
@@ -1644,15 +1630,15 @@
         <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>-3.0916000000000001</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>-60.0261</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1668,7 +1654,7 @@
         <v>10</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>126</v>
@@ -1680,7 +1666,7 @@
         <v>11</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>48</v>
@@ -1688,7 +1674,7 @@
       <c r="Q12" s="1">
         <v>8747</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="3">
         <v>33</v>
       </c>
     </row>
@@ -1700,15 +1686,15 @@
         <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>-3.0945</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>-60.024999999999999</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1724,7 +1710,7 @@
         <v>21</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>126</v>
@@ -1736,7 +1722,7 @@
         <v>14</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>50</v>
@@ -1744,7 +1730,7 @@
       <c r="Q13" s="1">
         <v>6162</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="3">
         <v>21</v>
       </c>
     </row>
@@ -1756,15 +1742,15 @@
         <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>-12.9748</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
         <v>-38.5124</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1777,10 +1763,10 @@
         <v>54</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>126</v>
@@ -1792,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>55</v>
@@ -1800,7 +1786,7 @@
       <c r="Q14" s="1">
         <v>8843</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1812,15 +1798,15 @@
         <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="E15" s="3">
         <v>-3.7319</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="3">
         <v>-38.499299999999998</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1836,7 +1822,7 @@
         <v>21</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>126</v>
@@ -1848,7 +1834,7 @@
         <v>14</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>59</v>
@@ -1856,7 +1842,7 @@
       <c r="Q15" s="1">
         <v>5526</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R15" s="3">
         <v>32</v>
       </c>
     </row>
@@ -1868,15 +1854,15 @@
         <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="E16" s="3">
         <v>-8.1227</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="3">
         <v>-34.9026</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1889,10 +1875,10 @@
         <v>62</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>126</v>
@@ -1904,7 +1890,7 @@
         <v>11</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>63</v>
@@ -1912,7 +1898,7 @@
       <c r="Q16" s="1">
         <v>5949</v>
       </c>
-      <c r="R16" s="5">
+      <c r="R16" s="3">
         <v>18</v>
       </c>
     </row>
@@ -1924,15 +1910,15 @@
         <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>-5.8403999999999998</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="3">
         <v>-35.206499999999998</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1948,7 +1934,7 @@
         <v>10</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>126</v>
@@ -1960,7 +1946,7 @@
         <v>22</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>67</v>
@@ -1968,7 +1954,7 @@
       <c r="Q17" s="1">
         <v>2470</v>
       </c>
-      <c r="R17" s="5">
+      <c r="R17" s="3">
         <v>10</v>
       </c>
     </row>
@@ -1980,15 +1966,15 @@
         <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="E18" s="3">
         <v>-25.4405</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="3">
         <v>-49.292299999999997</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -2001,10 +1987,10 @@
         <v>71</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>126</v>
@@ -2016,7 +2002,7 @@
         <v>14</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>72</v>
@@ -2024,7 +2010,7 @@
       <c r="Q18" s="1">
         <v>9146</v>
       </c>
-      <c r="R18" s="5">
+      <c r="R18" s="3">
         <v>29</v>
       </c>
     </row>
@@ -2036,15 +2022,15 @@
         <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" s="5">
+      <c r="E19" s="3">
         <v>-23.304400000000001</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="3">
         <v>-51.1691</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -2060,7 +2046,7 @@
         <v>10</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>126</v>
@@ -2072,7 +2058,7 @@
         <v>11</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>75</v>
@@ -2080,7 +2066,7 @@
       <c r="Q19" s="1">
         <v>8407</v>
       </c>
-      <c r="R19" s="5">
+      <c r="R19" s="3">
         <v>32</v>
       </c>
     </row>
@@ -2092,15 +2078,15 @@
         <v>76</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E20" s="5">
+      <c r="E20" s="3">
         <v>-27.594899999999999</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="3">
         <v>-48.548200000000001</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -2113,10 +2099,10 @@
         <v>78</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>126</v>
@@ -2128,7 +2114,7 @@
         <v>11</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>79</v>
@@ -2136,7 +2122,7 @@
       <c r="Q20" s="1">
         <v>1675</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="3">
         <v>18</v>
       </c>
     </row>
@@ -2148,15 +2134,15 @@
         <v>80</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E21" s="5">
+      <c r="E21" s="3">
         <v>-26.304400000000001</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="3">
         <v>-48.8461</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -2169,10 +2155,10 @@
         <v>81</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>126</v>
@@ -2184,7 +2170,7 @@
         <v>22</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>82</v>
@@ -2192,7 +2178,7 @@
       <c r="Q21" s="1">
         <v>8970</v>
       </c>
-      <c r="R21" s="5">
+      <c r="R21" s="3">
         <v>18</v>
       </c>
     </row>
@@ -2204,15 +2190,15 @@
         <v>83</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E22" s="5">
+      <c r="E22" s="3">
         <v>-16.6799</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="3">
         <v>-49.255000000000003</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -2225,10 +2211,10 @@
         <v>86</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>126</v>
@@ -2240,7 +2226,7 @@
         <v>11</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>87</v>
@@ -2248,7 +2234,7 @@
       <c r="Q22" s="1">
         <v>6572</v>
       </c>
-      <c r="R22" s="5">
+      <c r="R22" s="3">
         <v>18</v>
       </c>
     </row>
@@ -2260,15 +2246,15 @@
         <v>88</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="5">
+      <c r="E23" s="3">
         <v>-20.4697</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="3">
         <v>-54.620100000000001</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -2281,10 +2267,10 @@
         <v>90</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>126</v>
@@ -2296,7 +2282,7 @@
         <v>22</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>91</v>
@@ -2304,7 +2290,7 @@
       <c r="Q23" s="1">
         <v>3514</v>
       </c>
-      <c r="R23" s="5">
+      <c r="R23" s="3">
         <v>4</v>
       </c>
     </row>
@@ -2316,15 +2302,15 @@
         <v>92</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="E24" s="3">
         <v>-15.569599999999999</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="3">
         <v>-56.073500000000003</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -2340,7 +2326,7 @@
         <v>21</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>126</v>
@@ -2352,7 +2338,7 @@
         <v>14</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>95</v>
@@ -2360,7 +2346,7 @@
       <c r="Q24" s="1">
         <v>4311</v>
       </c>
-      <c r="R24" s="5">
+      <c r="R24" s="3">
         <v>20</v>
       </c>
     </row>
@@ -2372,15 +2358,15 @@
         <v>96</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E25" s="5">
+      <c r="E25" s="3">
         <v>-15.815</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="3">
         <v>-47.897599999999997</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -2396,7 +2382,7 @@
         <v>21</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>126</v>
@@ -2408,7 +2394,7 @@
         <v>14</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>99</v>
@@ -2416,7 +2402,7 @@
       <c r="Q25" s="1">
         <v>3851</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R25" s="3">
         <v>33</v>
       </c>
     </row>
@@ -2428,15 +2414,15 @@
         <v>100</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="5">
+      <c r="E26" s="3">
         <v>-22.8964</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="3">
         <v>-43.124600000000001</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -2452,7 +2438,7 @@
         <v>21</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>126</v>
@@ -2464,7 +2450,7 @@
         <v>11</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>103</v>
@@ -2472,7 +2458,7 @@
       <c r="Q26" s="1">
         <v>526</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="3">
         <v>9</v>
       </c>
     </row>
@@ -2484,15 +2470,15 @@
         <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E27" s="5">
+      <c r="E27" s="3">
         <v>-22.903500000000001</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="3">
         <v>-43.1768</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -2508,7 +2494,7 @@
         <v>21</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>126</v>
@@ -2520,7 +2506,7 @@
         <v>11</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>106</v>
@@ -2528,7 +2514,7 @@
       <c r="Q27" s="1">
         <v>9245</v>
       </c>
-      <c r="R27" s="5">
+      <c r="R27" s="3">
         <v>20</v>
       </c>
     </row>
@@ -2540,15 +2526,15 @@
         <v>107</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="E28" s="3">
         <v>-23.001100000000001</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="3">
         <v>-43.365400000000001</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -2561,10 +2547,10 @@
         <v>105</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>126</v>
@@ -2576,7 +2562,7 @@
         <v>14</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>108</v>
@@ -2584,7 +2570,7 @@
       <c r="Q28" s="1">
         <v>8592</v>
       </c>
-      <c r="R28" s="5">
+      <c r="R28" s="3">
         <v>13</v>
       </c>
     </row>
@@ -2596,15 +2582,15 @@
         <v>109</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E29" s="5">
+      <c r="E29" s="3">
         <v>-22.523399999999999</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="3">
         <v>-44.104900000000001</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -2617,10 +2603,10 @@
         <v>110</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>126</v>
@@ -2632,7 +2618,7 @@
         <v>22</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>111</v>
@@ -2640,7 +2626,7 @@
       <c r="Q29" s="1">
         <v>1146</v>
       </c>
-      <c r="R29" s="5">
+      <c r="R29" s="3">
         <v>11</v>
       </c>
     </row>
@@ -2652,15 +2638,15 @@
         <v>112</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E30" s="5">
+      <c r="E30" s="3">
         <v>-2.5297000000000001</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="3">
         <v>-44.302799999999998</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -2673,10 +2659,10 @@
         <v>114</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>126</v>
@@ -2688,7 +2674,7 @@
         <v>11</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>115</v>
@@ -2696,7 +2682,7 @@
       <c r="Q30" s="1">
         <v>5761</v>
       </c>
-      <c r="R30" s="5">
+      <c r="R30" s="3">
         <v>29</v>
       </c>
     </row>
@@ -2708,15 +2694,15 @@
         <v>116</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31" s="5">
+      <c r="E31" s="3">
         <v>-5.0826000000000002</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="3">
         <v>-42.802199999999999</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -2729,10 +2715,10 @@
         <v>118</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>126</v>
@@ -2744,7 +2730,7 @@
         <v>22</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>119</v>
@@ -2752,7 +2738,7 @@
       <c r="Q31" s="1">
         <v>6278</v>
       </c>
-      <c r="R31" s="5">
+      <c r="R31" s="3">
         <v>9</v>
       </c>
     </row>
@@ -2760,1158 +2746,4 @@
   <autoFilter ref="A1:R31" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A394E2EF-EE1A-4307-AC76-73BBB7BE3543}">
-  <dimension ref="A1:K31"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1001</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="4">
-        <v>-235439</v>
-      </c>
-      <c r="F2" s="4">
-        <v>-466410</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <f>E2/10000</f>
-        <v>-23.543900000000001</v>
-      </c>
-      <c r="K2">
-        <f>F2/10000</f>
-        <v>-46.640999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>1002</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="4">
-        <v>-235615</v>
-      </c>
-      <c r="F3" s="4">
-        <v>-466563</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3">
-        <f>E3/10000</f>
-        <v>-23.561499999999999</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K31" si="0">F3/10000</f>
-        <v>-46.656300000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>1003</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="4">
-        <v>-229056</v>
-      </c>
-      <c r="F4" s="4">
-        <v>-470608</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J31" si="1">E4/10000</f>
-        <v>-22.9056</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>-47.0608</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>1004</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="4">
-        <v>-239675</v>
-      </c>
-      <c r="F5" s="4">
-        <v>-463343</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
-        <v>-23.967500000000001</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>-46.334299999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>1005</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="4">
-        <v>-211775</v>
-      </c>
-      <c r="F6" s="4">
-        <v>-478208</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>-21.177499999999998</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>-47.820799999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>1006</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="4">
-        <v>-236914</v>
-      </c>
-      <c r="F7" s="4">
-        <v>-465646</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
-        <v>-23.691400000000002</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>-46.564599999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>2001</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="4">
-        <v>-199386</v>
-      </c>
-      <c r="F8" s="4">
-        <v>-439334</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
-        <v>-19.938600000000001</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>-43.933399999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>2002</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="4">
-        <v>-189145</v>
-      </c>
-      <c r="F9" s="4">
-        <v>-482754</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>-18.9145</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>-48.275399999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>2003</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="4">
-        <v>-199381</v>
-      </c>
-      <c r="F10" s="4">
-        <v>-440366</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>-19.938099999999999</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>-44.0366</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>3001</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E11" s="4">
-        <v>-99747</v>
-      </c>
-      <c r="F11" s="4">
-        <v>-678249</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
-        <v>-9.9747000000000003</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>-67.8249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>3002</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="4">
-        <v>-30916</v>
-      </c>
-      <c r="F12" s="4">
-        <v>-600261</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="1"/>
-        <v>-3.0916000000000001</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>-60.0261</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>3003</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" s="4">
-        <v>-30945</v>
-      </c>
-      <c r="F13" s="4">
-        <v>-600250</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>-3.0945</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>-60.024999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>4001</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" s="4">
-        <v>-129748</v>
-      </c>
-      <c r="F14" s="4">
-        <v>-385124</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>-12.9748</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>-38.5124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>4002</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E15" s="4">
-        <v>-37319</v>
-      </c>
-      <c r="F15" s="4">
-        <v>-384993</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
-        <v>-3.7319</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>-38.499299999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>4003</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" s="4">
-        <v>-81227</v>
-      </c>
-      <c r="F16" s="4">
-        <v>-349026</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>-8.1227</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>-34.9026</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>4004</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E17" s="4">
-        <v>-58404</v>
-      </c>
-      <c r="F17" s="4">
-        <v>-352065</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
-        <v>-5.8403999999999998</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>-35.206499999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>5001</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E18" s="4">
-        <v>-254405</v>
-      </c>
-      <c r="F18" s="4">
-        <v>-492923</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="1"/>
-        <v>-25.4405</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>-49.292299999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>5002</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" s="4">
-        <v>-233044</v>
-      </c>
-      <c r="F19" s="4">
-        <v>-511691</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
-        <v>-23.304400000000001</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>-51.1691</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>5003</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E20" s="4">
-        <v>-275949</v>
-      </c>
-      <c r="F20" s="4">
-        <v>-485482</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
-        <v>-27.594899999999999</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>-48.548200000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>5004</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E21" s="4">
-        <v>-263044</v>
-      </c>
-      <c r="F21" s="4">
-        <v>-488461</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="1"/>
-        <v>-26.304400000000001</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>-48.8461</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>6001</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E22" s="4">
-        <v>-166799</v>
-      </c>
-      <c r="F22" s="4">
-        <v>-492550</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="1"/>
-        <v>-16.6799</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>-49.255000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
-        <v>6002</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="4">
-        <v>-204697</v>
-      </c>
-      <c r="F23" s="4">
-        <v>-546201</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
-        <v>-20.4697</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>-54.620100000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
-        <v>6003</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E24" s="4">
-        <v>-155696</v>
-      </c>
-      <c r="F24" s="4">
-        <v>-560735</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="1"/>
-        <v>-15.569599999999999</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>-56.073500000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>6004</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E25" s="4">
-        <v>-158150</v>
-      </c>
-      <c r="F25" s="4">
-        <v>-478976</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="1"/>
-        <v>-15.815</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>-47.897599999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>7001</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="4">
-        <v>-228964</v>
-      </c>
-      <c r="F26" s="4">
-        <v>-431246</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="1"/>
-        <v>-22.8964</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
-        <v>-43.124600000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
-        <v>7002</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E27" s="4">
-        <v>-229035</v>
-      </c>
-      <c r="F27" s="4">
-        <v>-431768</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="1"/>
-        <v>-22.903500000000001</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>-43.1768</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
-        <v>7003</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E28" s="4">
-        <v>-230011</v>
-      </c>
-      <c r="F28" s="4">
-        <v>-433654</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
-        <v>-23.001100000000001</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>-43.365400000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
-        <v>7004</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E29" s="4">
-        <v>-225234</v>
-      </c>
-      <c r="F29" s="4">
-        <v>-441049</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="1"/>
-        <v>-22.523399999999999</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
-        <v>-44.104900000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
-        <v>8001</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="E30" s="4">
-        <v>-25297</v>
-      </c>
-      <c r="F30" s="4">
-        <v>-443028</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="1"/>
-        <v>-2.5297000000000001</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="0"/>
-        <v>-44.302799999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
-        <v>8002</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31" s="4">
-        <v>-50826</v>
-      </c>
-      <c r="F31" s="4">
-        <v>-428022</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="1"/>
-        <v>-5.0826000000000002</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
-        <v>-42.802199999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Enhance data processing with duplicate column resolution
- Added a new function `resolve_duplicate_columns` to handle duplicate columns in DataFrames with various strategies (rename, keep_first, keep_last, drop).
- Integrated the duplicate column resolution in the `post_process_table` function of the budget reader to ensure data integrity.
- Updated the result concatenation logic in `append_and_save_results` and `orchestrate_budget_reader` to use the new `concat_dataframes` function for better handling of missing data.
- Modified the output reports to reflect updated statistics and corrected values.
</commit_message>
<xml_diff>
--- a/data/inputs/agencias/BASE_AGENCIAS.xlsx
+++ b/data/inputs/agencias/BASE_AGENCIAS.xlsx
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: Update settings and validation functions for improved data processing and output management
</commit_message>
<xml_diff>
--- a/data/inputs/agencias/BASE_AGENCIAS.xlsx
+++ b/data/inputs/agencias/BASE_AGENCIAS.xlsx
@@ -882,15 +882,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -902,6 +893,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1211,40 +1211,40 @@
     <col min="21" max="21" width="14.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="6" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="8" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="7" t="s">
         <v>243</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Update budget and validation scripts; add new data files and remove obsolete ones
</commit_message>
<xml_diff>
--- a/data/inputs/agencias/BASE_AGENCIAS.xlsx
+++ b/data/inputs/agencias/BASE_AGENCIAS.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/agencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F3465D4-2E89-458C-B19D-967CA1312C2A}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF8A583F-3BDA-4178-BB19-67D2D6BF484D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$2:$U$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$2:$U$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="255">
   <si>
     <t>CD_PONTO</t>
   </si>
@@ -771,6 +772,39 @@
   </si>
   <si>
     <t>QUADRO DE FUNCIONÁRIOS</t>
+  </si>
+  <si>
+    <t>Itaú Osasco Centro</t>
+  </si>
+  <si>
+    <t>Rua Antônio Agú, 685 – Centro</t>
+  </si>
+  <si>
+    <t>06010-000</t>
+  </si>
+  <si>
+    <t>Osasco</t>
+  </si>
+  <si>
+    <t>2018-08</t>
+  </si>
+  <si>
+    <t>Itaú Santa Cruz do Sul Centro</t>
+  </si>
+  <si>
+    <t>Rua Marechal Floriano, 215 – Centro</t>
+  </si>
+  <si>
+    <t>96810-010</t>
+  </si>
+  <si>
+    <t>Santa Cruz do Sul</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>2018-05</t>
   </si>
 </sst>
 </file>
@@ -871,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -902,6 +936,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1313,86 +1350,86 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1001</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3">
-        <v>-23.543900000000001</v>
-      </c>
-      <c r="K3" s="3">
-        <v>-46.640999999999998</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="J3" s="11">
+        <v>-23.532900000000001</v>
+      </c>
+      <c r="K3" s="11">
+        <v>-46.791600000000003</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T3" s="1">
-        <v>8119</v>
-      </c>
-      <c r="U3" s="3">
-        <v>13</v>
+      <c r="Q3" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="T3" s="11">
+        <v>5200</v>
+      </c>
+      <c r="U3" s="11">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>3893</v>
+        <v>1001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
@@ -1404,13 +1441,13 @@
         <v>5</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J4" s="3">
-        <v>-23.561499999999999</v>
+        <v>-23.543900000000001</v>
       </c>
       <c r="K4" s="3">
-        <v>-46.656300000000002</v>
+        <v>-46.640999999999998</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>191</v>
@@ -1422,45 +1459,45 @@
         <v>120</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="1">
+        <v>8119</v>
+      </c>
+      <c r="U4" s="3">
         <v>13</v>
       </c>
-      <c r="T4" s="1">
-        <v>4126</v>
-      </c>
-      <c r="U4" s="3">
-        <v>34</v>
-      </c>
     </row>
-    <row r="5" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3149</v>
+        <v>3893</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
@@ -1472,16 +1509,16 @@
         <v>19</v>
       </c>
       <c r="J5" s="3">
-        <v>-22.9056</v>
+        <v>-23.561499999999999</v>
       </c>
       <c r="K5" s="3">
-        <v>-47.0608</v>
+        <v>-46.656300000000002</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>120</v>
@@ -1490,42 +1527,42 @@
         <v>229</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="T5" s="1">
-        <v>2706</v>
+        <v>4126</v>
       </c>
       <c r="U5" s="3">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>1004</v>
+        <v>3149</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>6</v>
@@ -1534,63 +1571,63 @@
         <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="J6" s="3">
-        <v>-23.967500000000001</v>
+        <v>-22.9056</v>
       </c>
       <c r="K6" s="3">
-        <v>-46.334299999999999</v>
+        <v>-47.0608</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>120</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="T6" s="1">
-        <v>6257</v>
+        <v>2706</v>
       </c>
       <c r="U6" s="3">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>6</v>
@@ -1602,60 +1639,60 @@
         <v>8</v>
       </c>
       <c r="J7" s="3">
-        <v>-21.177499999999998</v>
+        <v>-23.967500000000001</v>
       </c>
       <c r="K7" s="3">
-        <v>-47.820799999999998</v>
+        <v>-46.334299999999999</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T7" s="1">
-        <v>4251</v>
+        <v>6257</v>
       </c>
       <c r="U7" s="3">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>167</v>
+        <v>1005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
@@ -1667,16 +1704,16 @@
         <v>8</v>
       </c>
       <c r="J8" s="3">
-        <v>-23.691400000000002</v>
+        <v>-21.177499999999998</v>
       </c>
       <c r="K8" s="3">
-        <v>-46.564599999999999</v>
+        <v>-47.820799999999998</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>119</v>
@@ -1685,107 +1722,107 @@
         <v>234</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>196</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="T8" s="1">
-        <v>4520</v>
+        <v>4251</v>
       </c>
       <c r="U8" s="3">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>2001</v>
+        <v>167</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J9" s="3">
-        <v>-19.938600000000001</v>
+        <v>-23.691400000000002</v>
       </c>
       <c r="K9" s="3">
-        <v>-43.933399999999999</v>
+        <v>-46.564599999999999</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>119</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="T9" s="1">
-        <v>2244</v>
+        <v>4520</v>
       </c>
       <c r="U9" s="3">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>29</v>
@@ -1794,40 +1831,40 @@
         <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="J10" s="3">
-        <v>-18.9145</v>
+        <v>-19.938600000000001</v>
       </c>
       <c r="K10" s="3">
-        <v>-48.275399999999998</v>
+        <v>-43.933399999999999</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>119</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="T10" s="1">
-        <v>3384</v>
+        <v>2244</v>
       </c>
       <c r="U10" s="3">
         <v>40</v>
@@ -1835,22 +1872,22 @@
     </row>
     <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>29</v>
@@ -1862,13 +1899,13 @@
         <v>8</v>
       </c>
       <c r="J11" s="3">
-        <v>-19.938099999999999</v>
+        <v>-18.9145</v>
       </c>
       <c r="K11" s="3">
-        <v>-44.0366</v>
+        <v>-48.275399999999998</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>124</v>
@@ -1877,169 +1914,169 @@
         <v>119</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="T11" s="1">
-        <v>7564</v>
+        <v>3384</v>
       </c>
       <c r="U11" s="3">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>3001</v>
+        <v>2003</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>198</v>
+        <v>8</v>
       </c>
       <c r="J12" s="3">
-        <v>-9.9747000000000003</v>
+        <v>-19.938099999999999</v>
       </c>
       <c r="K12" s="3">
-        <v>-67.8249</v>
+        <v>-44.0366</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="T12" s="1">
-        <v>2589</v>
+        <v>7564</v>
       </c>
       <c r="U12" s="3">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="J13" s="3">
-        <v>-3.0916000000000001</v>
+        <v>-9.9747000000000003</v>
       </c>
       <c r="K13" s="3">
-        <v>-60.0261</v>
+        <v>-67.8249</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>120</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>193</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="T13" s="1">
-        <v>8747</v>
+        <v>2589</v>
       </c>
       <c r="U13" s="3">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>213</v>
@@ -2054,78 +2091,78 @@
         <v>39</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J14" s="3">
-        <v>-3.0945</v>
+        <v>-3.0916000000000001</v>
       </c>
       <c r="K14" s="3">
-        <v>-60.024999999999999</v>
+        <v>-60.0261</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>124</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>193</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="T14" s="1">
-        <v>6162</v>
+        <v>8747</v>
       </c>
       <c r="U14" s="3">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>4001</v>
+        <v>3003</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>198</v>
+        <v>19</v>
       </c>
       <c r="J15" s="3">
-        <v>-12.9748</v>
+        <v>-3.0945</v>
       </c>
       <c r="K15" s="3">
-        <v>-38.5124</v>
+        <v>-60.024999999999999</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>191</v>
@@ -2140,57 +2177,57 @@
         <v>229</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>193</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="T15" s="1">
-        <v>8843</v>
+        <v>6162</v>
       </c>
       <c r="U15" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>4002</v>
+        <v>4001</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="J16" s="3">
-        <v>-3.7319</v>
+        <v>-12.9748</v>
       </c>
       <c r="K16" s="3">
-        <v>-38.499299999999998</v>
+        <v>-38.5124</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>191</v>
@@ -2199,243 +2236,243 @@
         <v>124</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>229</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>193</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="T16" s="1">
-        <v>5526</v>
+        <v>8843</v>
       </c>
       <c r="U16" s="3">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>4003</v>
+        <v>4002</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>198</v>
+        <v>19</v>
       </c>
       <c r="J17" s="3">
-        <v>-8.1227</v>
+        <v>-3.7319</v>
       </c>
       <c r="K17" s="3">
-        <v>-34.9026</v>
+        <v>-38.499299999999998</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="T17" s="1">
-        <v>5949</v>
+        <v>5526</v>
       </c>
       <c r="U17" s="3">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>4004</v>
+        <v>4003</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="J18" s="3">
-        <v>-5.8403999999999998</v>
+        <v>-8.1227</v>
       </c>
       <c r="K18" s="3">
-        <v>-35.206499999999998</v>
+        <v>-34.9026</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>232</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T18" s="1">
-        <v>2470</v>
+        <v>5949</v>
       </c>
       <c r="U18" s="3">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>5001</v>
+        <v>4004</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>198</v>
+        <v>8</v>
       </c>
       <c r="J19" s="3">
-        <v>-25.4405</v>
+        <v>-5.8403999999999998</v>
       </c>
       <c r="K19" s="3">
-        <v>-49.292299999999997</v>
+        <v>-35.206499999999998</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>195</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>193</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="T19" s="1">
-        <v>9146</v>
+        <v>2470</v>
       </c>
       <c r="U19" s="3">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>68</v>
@@ -2444,13 +2481,13 @@
         <v>67</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="J20" s="3">
-        <v>-23.304400000000001</v>
+        <v>-25.4405</v>
       </c>
       <c r="K20" s="3">
-        <v>-51.1691</v>
+        <v>-49.292299999999997</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>195</v>
@@ -2462,60 +2499,60 @@
         <v>119</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="T20" s="1">
-        <v>8407</v>
+        <v>9146</v>
       </c>
       <c r="U20" s="3">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>67</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>198</v>
+        <v>8</v>
       </c>
       <c r="J21" s="3">
-        <v>-27.594899999999999</v>
+        <v>-23.304400000000001</v>
       </c>
       <c r="K21" s="3">
-        <v>-48.548200000000001</v>
+        <v>-51.1691</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>195</v>
@@ -2524,7 +2561,7 @@
         <v>124</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>232</v>
@@ -2536,36 +2573,36 @@
         <v>237</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="T21" s="1">
-        <v>1675</v>
+        <v>8407</v>
       </c>
       <c r="U21" s="3">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>5004</v>
+        <v>5003</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>75</v>
@@ -2577,128 +2614,128 @@
         <v>198</v>
       </c>
       <c r="J22" s="3">
-        <v>-26.304400000000001</v>
+        <v>-27.594899999999999</v>
       </c>
       <c r="K22" s="3">
-        <v>-48.8461</v>
+        <v>-48.548200000000001</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>195</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>193</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="T22" s="1">
-        <v>8970</v>
+        <v>1675</v>
       </c>
       <c r="U22" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>6001</v>
+        <v>5004</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>198</v>
       </c>
       <c r="J23" s="3">
-        <v>-16.6799</v>
+        <v>-26.304400000000001</v>
       </c>
       <c r="K23" s="3">
-        <v>-49.255000000000003</v>
+        <v>-48.8461</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>195</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>119</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="T23" s="1">
-        <v>6572</v>
+        <v>8970</v>
       </c>
       <c r="U23" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>6002</v>
+        <v>6001</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>82</v>
@@ -2707,13 +2744,13 @@
         <v>198</v>
       </c>
       <c r="J24" s="3">
-        <v>-20.4697</v>
+        <v>-16.6799</v>
       </c>
       <c r="K24" s="3">
-        <v>-54.620100000000001</v>
+        <v>-49.255000000000003</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>124</v>
@@ -2722,113 +2759,113 @@
         <v>119</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="T24" s="1">
-        <v>3514</v>
+        <v>6572</v>
       </c>
       <c r="U24" s="3">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>6003</v>
+        <v>6002</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>82</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="J25" s="3">
-        <v>-15.569599999999999</v>
+        <v>-20.4697</v>
       </c>
       <c r="K25" s="3">
-        <v>-56.073500000000003</v>
+        <v>-54.620100000000001</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>192</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="T25" s="1">
-        <v>4311</v>
+        <v>3514</v>
       </c>
       <c r="U25" s="3">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>6004</v>
+        <v>6003</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>82</v>
@@ -2837,22 +2874,22 @@
         <v>19</v>
       </c>
       <c r="J26" s="3">
-        <v>-15.815</v>
+        <v>-15.569599999999999</v>
       </c>
       <c r="K26" s="3">
-        <v>-47.897599999999997</v>
+        <v>-56.073500000000003</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>12</v>
@@ -2861,101 +2898,101 @@
         <v>239</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="T26" s="1">
-        <v>3851</v>
+        <v>4311</v>
       </c>
       <c r="U26" s="3">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>7001</v>
+        <v>6004</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J27" s="3">
-        <v>-22.8964</v>
+        <v>-15.815</v>
       </c>
       <c r="K27" s="3">
-        <v>-43.124600000000001</v>
+        <v>-47.897599999999997</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>119</v>
       </c>
       <c r="O27" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="S27" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="T27" s="1">
-        <v>526</v>
+        <v>3851</v>
       </c>
       <c r="U27" s="3">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>7002</v>
+        <v>7001</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>99</v>
@@ -2967,19 +3004,19 @@
         <v>19</v>
       </c>
       <c r="J28" s="3">
-        <v>-22.903500000000001</v>
+        <v>-22.8964</v>
       </c>
       <c r="K28" s="3">
-        <v>-43.1768</v>
+        <v>-43.124600000000001</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>199</v>
@@ -2988,36 +3025,36 @@
         <v>9</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>196</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="T28" s="1">
-        <v>9245</v>
+        <v>526</v>
       </c>
       <c r="U28" s="3">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>7003</v>
+        <v>7002</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>103</v>
@@ -3029,13 +3066,13 @@
         <v>5</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>198</v>
+        <v>19</v>
       </c>
       <c r="J29" s="3">
-        <v>-23.001100000000001</v>
+        <v>-22.903500000000001</v>
       </c>
       <c r="K29" s="3">
-        <v>-43.365400000000001</v>
+        <v>-43.1768</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>195</v>
@@ -3047,45 +3084,45 @@
         <v>120</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>235</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T29" s="1">
-        <v>8592</v>
+        <v>9245</v>
       </c>
       <c r="U29" s="3">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>7004</v>
+        <v>7003</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>99</v>
@@ -3097,128 +3134,128 @@
         <v>198</v>
       </c>
       <c r="J30" s="3">
-        <v>-22.523399999999999</v>
+        <v>-23.001100000000001</v>
       </c>
       <c r="K30" s="3">
-        <v>-44.104900000000001</v>
+        <v>-43.365400000000001</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>195</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="T30" s="1">
-        <v>1146</v>
+        <v>8592</v>
       </c>
       <c r="U30" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>8001</v>
+        <v>7004</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>198</v>
       </c>
       <c r="J31" s="3">
-        <v>-2.5297000000000001</v>
+        <v>-22.523399999999999</v>
       </c>
       <c r="K31" s="3">
-        <v>-44.302799999999998</v>
+        <v>-44.104900000000001</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>119</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="T31" s="1">
-        <v>5761</v>
+        <v>1146</v>
       </c>
       <c r="U31" s="3">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>8002</v>
+        <v>8001</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>50</v>
@@ -3227,44 +3264,174 @@
         <v>198</v>
       </c>
       <c r="J32" s="3">
-        <v>-5.0826000000000002</v>
+        <v>-2.5297000000000001</v>
       </c>
       <c r="K32" s="3">
-        <v>-42.802199999999999</v>
+        <v>-44.302799999999998</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M32" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="T32" s="1">
+        <v>5761</v>
+      </c>
+      <c r="U32" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>8002</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J33" s="3">
+        <v>-5.0826000000000002</v>
+      </c>
+      <c r="K33" s="3">
+        <v>-42.802199999999999</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M33" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="S33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T32" s="1">
+      <c r="T33" s="1">
         <v>6278</v>
       </c>
-      <c r="U32" s="3">
+      <c r="U33" s="3">
         <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>605</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="3">
+        <v>-29.717600000000001</v>
+      </c>
+      <c r="K34" s="3">
+        <v>-52.427399999999999</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="T34" s="3">
+        <v>3100</v>
+      </c>
+      <c r="U34" s="3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U32" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:U34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:K1"/>
@@ -3272,4 +3439,279 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014EA6DB-8A17-4B4C-90CE-CF5BC0692047}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:U5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" t="s">
+        <v>225</v>
+      </c>
+      <c r="P1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>226</v>
+      </c>
+      <c r="R1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" t="s">
+        <v>190</v>
+      </c>
+      <c r="U1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>-23.532900000000001</v>
+      </c>
+      <c r="K2">
+        <v>-46.791600000000003</v>
+      </c>
+      <c r="L2" t="s">
+        <v>191</v>
+      </c>
+      <c r="M2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O2" t="s">
+        <v>199</v>
+      </c>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>230</v>
+      </c>
+      <c r="R2" t="s">
+        <v>196</v>
+      </c>
+      <c r="S2" t="s">
+        <v>248</v>
+      </c>
+      <c r="T2">
+        <v>5200</v>
+      </c>
+      <c r="U2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" t="s">
+        <v>118</v>
+      </c>
+      <c r="M4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" t="s">
+        <v>225</v>
+      </c>
+      <c r="P4" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>226</v>
+      </c>
+      <c r="R4" t="s">
+        <v>189</v>
+      </c>
+      <c r="S4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" t="s">
+        <v>190</v>
+      </c>
+      <c r="U4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>605</v>
+      </c>
+      <c r="B5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>-29.717600000000001</v>
+      </c>
+      <c r="K5">
+        <v>-52.427399999999999</v>
+      </c>
+      <c r="L5" t="s">
+        <v>195</v>
+      </c>
+      <c r="M5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O5" t="s">
+        <v>199</v>
+      </c>
+      <c r="P5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>230</v>
+      </c>
+      <c r="R5" t="s">
+        <v>196</v>
+      </c>
+      <c r="S5" t="s">
+        <v>254</v>
+      </c>
+      <c r="T5">
+        <v>3100</v>
+      </c>
+      <c r="U5">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add fuzzy matching functionality for constructor validation; update settings for merge options
</commit_message>
<xml_diff>
--- a/data/inputs/agencias/BASE_AGENCIAS.xlsx
+++ b/data/inputs/agencias/BASE_AGENCIAS.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/agencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF8A583F-3BDA-4178-BB19-67D2D6BF484D}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B1D1840-558B-4F3D-AC3C-9A5F35387F95}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$2:$U$34</definedName>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="255">
   <si>
     <t>CD_PONTO</t>
   </si>
@@ -928,6 +927,9 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -936,9 +938,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1249,29 +1248,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
       <c r="R1" s="5" t="s">
         <v>241</v>
       </c>
@@ -1351,67 +1350,67 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="8">
         <v>-23.532900000000001</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="8">
         <v>-46.791600000000003</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="8">
         <v>5200</v>
       </c>
-      <c r="U3" s="11">
+      <c r="U3" s="8">
         <v>18</v>
       </c>
     </row>
@@ -3439,279 +3438,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014EA6DB-8A17-4B4C-90CE-CF5BC0692047}">
-  <dimension ref="A1:U5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:U5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" t="s">
-        <v>128</v>
-      </c>
-      <c r="L1" t="s">
-        <v>118</v>
-      </c>
-      <c r="M1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" t="s">
-        <v>122</v>
-      </c>
-      <c r="O1" t="s">
-        <v>225</v>
-      </c>
-      <c r="P1" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>226</v>
-      </c>
-      <c r="R1" t="s">
-        <v>189</v>
-      </c>
-      <c r="S1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" t="s">
-        <v>190</v>
-      </c>
-      <c r="U1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F2" t="s">
-        <v>247</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>-23.532900000000001</v>
-      </c>
-      <c r="K2">
-        <v>-46.791600000000003</v>
-      </c>
-      <c r="L2" t="s">
-        <v>191</v>
-      </c>
-      <c r="M2" t="s">
-        <v>124</v>
-      </c>
-      <c r="N2" t="s">
-        <v>120</v>
-      </c>
-      <c r="O2" t="s">
-        <v>199</v>
-      </c>
-      <c r="P2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>230</v>
-      </c>
-      <c r="R2" t="s">
-        <v>196</v>
-      </c>
-      <c r="S2" t="s">
-        <v>248</v>
-      </c>
-      <c r="T2">
-        <v>5200</v>
-      </c>
-      <c r="U2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
-        <v>205</v>
-      </c>
-      <c r="F4" t="s">
-        <v>204</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>206</v>
-      </c>
-      <c r="J4" t="s">
-        <v>127</v>
-      </c>
-      <c r="K4" t="s">
-        <v>128</v>
-      </c>
-      <c r="L4" t="s">
-        <v>118</v>
-      </c>
-      <c r="M4" t="s">
-        <v>123</v>
-      </c>
-      <c r="N4" t="s">
-        <v>122</v>
-      </c>
-      <c r="O4" t="s">
-        <v>225</v>
-      </c>
-      <c r="P4" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>226</v>
-      </c>
-      <c r="R4" t="s">
-        <v>189</v>
-      </c>
-      <c r="S4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T4" t="s">
-        <v>190</v>
-      </c>
-      <c r="U4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>605</v>
-      </c>
-      <c r="B5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C5" t="s">
-        <v>250</v>
-      </c>
-      <c r="D5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E5" t="s">
-        <v>207</v>
-      </c>
-      <c r="F5" t="s">
-        <v>252</v>
-      </c>
-      <c r="G5" t="s">
-        <v>253</v>
-      </c>
-      <c r="H5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>-29.717600000000001</v>
-      </c>
-      <c r="K5">
-        <v>-52.427399999999999</v>
-      </c>
-      <c r="L5" t="s">
-        <v>195</v>
-      </c>
-      <c r="M5" t="s">
-        <v>124</v>
-      </c>
-      <c r="N5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O5" t="s">
-        <v>199</v>
-      </c>
-      <c r="P5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>230</v>
-      </c>
-      <c r="R5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S5" t="s">
-        <v>254</v>
-      </c>
-      <c r="T5">
-        <v>3100</v>
-      </c>
-      <c r="U5">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>